<commit_message>
Added T-cell pipeline. CIMR not included because of differing stain names in FCS files.
</commit_message>
<xml_diff>
--- a/Stanford.xlsx
+++ b/Stanford.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comp controls" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
-    <t>1349-1_A5_A05.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1349-1_A6_A06.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1369-1_A8_A08.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1369-1_A9_A09.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>1228-1_B1_B01.fcs</t>
   </si>
   <si>
@@ -222,9 +206,6 @@
     <t>1228-3_E3_E03.fcs</t>
   </si>
   <si>
-    <t>1228-1_A1_A01.FCS</t>
-  </si>
-  <si>
     <t>1369-1_C7_C07.fcs</t>
   </si>
   <si>
@@ -301,6 +282,21 @@
   </si>
   <si>
     <t>Compensation Controls_HLA DR Am Cyan-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>1228-1_A1_A01.fcs</t>
+  </si>
+  <si>
+    <t>1349-2_A5_A05.fcs</t>
+  </si>
+  <si>
+    <t>1349-3_A6_A06.fcs</t>
+  </si>
+  <si>
+    <t>1369-2_A8_A08.fcs</t>
+  </si>
+  <si>
+    <t>1369-3_A9_A09.fcs</t>
   </si>
 </sst>
 </file>
@@ -379,8 +375,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -407,11 +405,13 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,13 +743,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="6" width="10.33203125" customWidth="1"/>
@@ -758,7 +758,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -778,36 +778,36 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>18000</v>
@@ -824,13 +824,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>54000</v>
@@ -847,13 +847,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4">
         <v>2250</v>
@@ -871,10 +871,10 @@
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4">
         <v>27000</v>
@@ -886,27 +886,27 @@
         <v>33000</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1">
         <v>29785</v>
@@ -915,75 +915,75 @@
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D12" s="4">
         <v>22500</v>
@@ -1001,31 +1001,31 @@
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4">
         <v>22500</v>
@@ -1037,48 +1037,48 @@
         <v>27500</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G16" s="1">
         <v>23688</v>
@@ -1087,33 +1087,33 @@
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4">
         <v>6750</v>
@@ -1130,13 +1130,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D19" s="4">
         <v>13500</v>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1181,35 +1181,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1220,11 +1220,11 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1235,11 +1235,11 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1250,11 +1250,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1265,11 +1265,11 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1280,11 +1280,11 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1295,11 +1295,11 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1310,11 +1310,11 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1325,11 +1325,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1340,11 +1340,11 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1355,11 +1355,11 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1370,11 +1370,11 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1385,11 +1385,11 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1400,11 +1400,11 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1415,11 +1415,11 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1430,11 +1430,11 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1445,11 +1445,11 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1460,11 +1460,11 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1475,11 +1475,11 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1490,11 +1490,11 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1505,11 +1505,11 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1520,11 +1520,11 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1535,11 +1535,11 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -1550,11 +1550,11 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1565,11 +1565,11 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1580,11 +1580,11 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -1595,11 +1595,11 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1610,11 +1610,11 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1625,11 +1625,11 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1640,11 +1640,11 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1655,11 +1655,11 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1670,11 +1670,11 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1685,11 +1685,11 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1700,11 +1700,11 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1715,11 +1715,11 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -1730,11 +1730,11 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1745,11 +1745,11 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1760,11 +1760,11 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -1775,11 +1775,11 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1790,11 +1790,11 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1805,11 +1805,11 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -1820,11 +1820,11 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -1835,11 +1835,11 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1850,11 +1850,11 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1865,11 +1865,11 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -1884,6 +1884,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added munging script to create DC/mono/NK GatingSet. BSMS not included because it did not include CD56
</commit_message>
<xml_diff>
--- a/Stanford.xlsx
+++ b/Stanford.xlsx
@@ -62,14 +62,6 @@
     <t>1228-1_D1_D01.fcs</t>
   </si>
   <si>
-    <t>1228-2_D1_D02.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1228-3_D1_D03.fcs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>1349-1_D4_D04.fcs</t>
   </si>
   <si>
@@ -297,6 +289,12 @@
   </si>
   <si>
     <t>1369-3_A9_A09.fcs</t>
+  </si>
+  <si>
+    <t>1228-2_D2_D02.fcs</t>
+  </si>
+  <si>
+    <t>1228-3_D3_D03.fcs</t>
   </si>
 </sst>
 </file>
@@ -758,7 +756,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -778,36 +776,36 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4">
         <v>18000</v>
@@ -824,13 +822,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
         <v>54000</v>
@@ -847,13 +845,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" s="4">
         <v>2250</v>
@@ -871,10 +869,10 @@
     <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" s="4">
         <v>27000</v>
@@ -886,27 +884,27 @@
         <v>33000</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1">
         <v>29785</v>
@@ -915,75 +913,75 @@
     <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="4">
         <v>22500</v>
@@ -1001,31 +999,31 @@
     <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="4">
         <v>22500</v>
@@ -1037,48 +1035,48 @@
         <v>27500</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G16" s="1">
         <v>23688</v>
@@ -1087,33 +1085,33 @@
     <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4">
         <v>6750</v>
@@ -1130,13 +1128,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" s="4">
         <v>13500</v>
@@ -1167,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1181,35 +1179,35 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1220,11 +1218,11 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1235,11 +1233,11 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1250,11 +1248,11 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1265,11 +1263,11 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1280,11 +1278,11 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1295,11 +1293,11 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1310,11 +1308,11 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1325,11 +1323,11 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1344,7 +1342,7 @@
       </c>
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1359,7 +1357,7 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1374,7 +1372,7 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1389,7 +1387,7 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1400,11 +1398,11 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1415,11 +1413,11 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1434,7 +1432,7 @@
       </c>
       <c r="B19" s="8"/>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1445,11 +1443,11 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1464,7 +1462,7 @@
       </c>
       <c r="B21" s="8"/>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1475,11 +1473,11 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1494,7 +1492,7 @@
       </c>
       <c r="B23" s="8"/>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1509,7 +1507,7 @@
       </c>
       <c r="B24" s="8"/>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1524,7 +1522,7 @@
       </c>
       <c r="B25" s="8"/>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1539,7 +1537,7 @@
       </c>
       <c r="B26" s="8"/>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -1554,7 +1552,7 @@
       </c>
       <c r="B27" s="8"/>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1565,11 +1563,11 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1580,11 +1578,11 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -1599,7 +1597,7 @@
       </c>
       <c r="B30" s="8"/>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1614,7 +1612,7 @@
       </c>
       <c r="B31" s="8"/>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1625,11 +1623,11 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1640,11 +1638,11 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1655,11 +1653,11 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1670,11 +1668,11 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -1685,11 +1683,11 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1700,11 +1698,11 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1715,11 +1713,11 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -1730,11 +1728,11 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1745,11 +1743,11 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1760,11 +1758,11 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -1775,11 +1773,11 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1790,11 +1788,11 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1805,11 +1803,11 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D44">
         <v>2</v>
@@ -1820,11 +1818,11 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D45">
         <v>3</v>
@@ -1835,11 +1833,11 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1850,11 +1848,11 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1865,11 +1863,11 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D48">
         <v>3</v>

</xml_diff>